<commit_message>
finish app development. remember: pyinstaller *.py -F --windowed to compile correctly
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thebr\Documents\excel_merger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024BAAF1-509B-47AD-B3D2-8EF91526F281}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3BE2CC2-0275-47D1-A5AE-BDCAFC48329F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6750" yWindow="2115" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{9CC0E6A4-3BC7-400A-B043-154BE2A44F33}"/>
+    <workbookView xWindow="6750" yWindow="2115" windowWidth="21600" windowHeight="11385" xr2:uid="{9CC0E6A4-3BC7-400A-B043-154BE2A44F33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3DA04B9-800A-4B38-AB35-5022F83F6C7A}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="A1:I28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,28 +493,28 @@
         <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1309,8 +1309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0D0EC1F-C72A-45E2-9C9C-BD0EFDED9413}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>